<commit_message>
Continuation de la documentation
</commit_message>
<xml_diff>
--- a/Docs/Analyse_Sanguine/Chemin critique.xlsx
+++ b/Docs/Analyse_Sanguine/Chemin critique.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ecole\Projet Final\Rooftop\Docs\Analyse_Sanguine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13240EE2-329C-4615-B5BD-2912F271654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A393D-A99A-4DEE-A2E6-550431C757AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7454C503-1B9C-4864-A7C2-5D0980A5147F}"/>
   </bookViews>
   <sheets>
     <sheet name="UseCase" sheetId="1" r:id="rId1"/>
-    <sheet name="Dépendance" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,8 +24,281 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>KarlAdmin</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{4C6C3528-C6C5-4785-8DF5-E2F10DD4F5A4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>API:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(En dev)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+L'avancement du API a bien avancée durant la semaine et celui-ci est fonctionnel, ainsi nous avons atteint ce que nous nous attendions de faire cette semaine</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{3FEBE9FA-5DD3-43A2-908D-646E354904C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">API: (Terminé)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Le travail était en moyenne très bien, les interfaces pour les controlleurs étaient bien, cependant quelques inconvénients ont été rencontrés durant l'ajout de seed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{2216F8CD-579D-4A6C-8028-1DAC6FF3989F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Créer la requête: (En dev)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Même si l'avancement du cas d'utilisation est relativement lent, le formulaire reste créer et le cas d'utilisation à permis à Maxime d'apprendre à faire des components react-native, ainsi le temps prit peut être justifié à cause de l'apprentissage qui venait avec.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{CE14D2F1-2A0A-4512-B04A-B6D19A7E5CBF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Créer la requête: (En dev)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La création du formulaire est fonctionnel, même s'il n'est pas terminé, une requête peut belle et bien être créé. Certaine type de test ne sont pas 100% fonctionnel, mais la majorité reste finit.
+L'excès de temps vient surtout du fait que le nombre de test ont clairement été sous-estimé de notre part, ainsi nous aurions dû prévoir plus de temps pour conclure la tâche.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{2D2B52A4-1255-4B7F-8805-DD8BAC12CC90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Créer le dossier: (En dev)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Le travail effectué sur la création de requête était très peu productive cette semaine. Le temps prit était énorme en comparaison au travail qui a été effectué (seulement le visuel). La lenteur est venu principalement du bouton qui amène au formulaire.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{7F1A0994-31F2-4C37-BCC3-3180BF0D1089}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Créer le dossier: (Terminé)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>L'avancement fait cette semaine sur la création de dossier était beaucoup plus productif cette semaine. Le formulaire a pu être terminé et même si le temps a été dépassé 2h45, l'avancement fait a été plus rapide qu'auparavant.
+De cette manière, l'excès de temps peut être vu à cause des problèmes avec l'accès au API qui est arrivé dans ce cas d'utilisation. Le bouton pour la création reste la cause principale de l'excès de temps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{A73F9D2D-BC66-4052-B833-9C65B10298C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rechercher un dossier: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Le cas d'utilisation a été fait dans des délais décent et respectait le temps que nous nous attendions. 
+Il n'y a pas eu de problème majeur qui a été rencontré et allongé le temps du cas.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{56C20E2C-26D6-4703-9F37-34B7B7749CAF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Modifier un dossier: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+La modification du dossier a été un cas d'utilisation qui c'est très bien déroulé. La durée a été dans les temps que nous avons prédis et il restait du temps si nous avons rencontré plus de problème.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{507B292C-E225-4152-B3E6-95B1D6E65C48}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>API Test: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Les test de l'API ont été terminés dans un délais de temps relativement faible tout en étant fonctionnel dans la très grande majorité.
+Ainsi, ses cas d'utilisations ont été terminés dans un délais que nous nous attendions.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{BF71BB93-A715-4EAF-863C-587AA0FD27DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Imprimer Requête: (En dev)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Il est difficile de vraiment expliquer une avancement, car il n'y a eu aucune avancée concrète dans le développement, mais plutôt une avancée dans les connaissances pour réaliser le développement dans les prochaines semaines.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -125,22 +397,13 @@
   </si>
   <si>
     <t>Temps Rel. s5</t>
-  </si>
-  <si>
-    <t>Aucun</t>
-  </si>
-  <si>
-    <t>Dépendence Id</t>
-  </si>
-  <si>
-    <t>9, 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +425,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -370,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -387,25 +669,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,11 +991,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5812C443-2D11-4192-ADEE-E8DB4E96BFCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5812C443-2D11-4192-ADEE-E8DB4E96BFCE}">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,10 +1047,14 @@
         <v>1.5</v>
       </c>
       <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="12"/>
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
@@ -790,14 +1066,18 @@
       <c r="D4" s="9">
         <v>2</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="12">
         <v>1.5</v>
       </c>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="14"/>
+      <c r="F4" s="12">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -809,14 +1089,18 @@
       <c r="D5" s="9">
         <v>2</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <v>1.5</v>
       </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="14"/>
+      <c r="F5" s="12">
+        <v>0</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
@@ -828,14 +1112,18 @@
       <c r="D6" s="9">
         <v>6</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="12">
         <v>1.5</v>
       </c>
-      <c r="F6" s="13">
-        <v>3.75</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="14"/>
+      <c r="F6" s="12">
+        <v>4.25</v>
+      </c>
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
@@ -847,14 +1135,18 @@
       <c r="D7" s="9">
         <v>6</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <v>1.5</v>
       </c>
-      <c r="F7" s="13">
-        <v>3.75</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="14"/>
+      <c r="F7" s="12">
+        <v>4.25</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
+      <c r="H7" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
@@ -866,14 +1158,18 @@
       <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="12">
         <v>1.5</v>
       </c>
-      <c r="F8" s="13">
-        <v>0</v>
-      </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="14"/>
+      <c r="F8" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
@@ -885,14 +1181,14 @@
       <c r="D9" s="9">
         <v>20</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <v>10.5</v>
       </c>
-      <c r="F9" s="13">
-        <v>7.65</v>
+      <c r="F9" s="14">
+        <v>10.9</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="14"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
@@ -904,14 +1200,14 @@
       <c r="D10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <v>2.5</v>
       </c>
-      <c r="F10" s="13">
-        <v>1.5</v>
+      <c r="F10" s="12">
+        <v>2</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="14"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
@@ -923,14 +1219,14 @@
       <c r="D11" s="9">
         <v>7</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="12">
         <v>2.5</v>
       </c>
-      <c r="F11" s="13">
-        <v>1.5</v>
+      <c r="F11" s="12">
+        <v>6.75</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="14"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
@@ -942,14 +1238,18 @@
       <c r="D12" s="9">
         <v>20</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="12">
         <v>9.5</v>
       </c>
-      <c r="F12" s="15">
-        <v>12.5</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="14"/>
+      <c r="F12" s="14">
+        <v>13.25</v>
+      </c>
+      <c r="G12" s="14">
+        <v>0</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
@@ -961,14 +1261,14 @@
       <c r="D13" s="9">
         <v>15</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="12">
         <v>11.5</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <v>1.1499999999999999</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
@@ -980,14 +1280,14 @@
       <c r="D14" s="9">
         <v>6</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>4.5</v>
       </c>
-      <c r="F14" s="15">
-        <v>2.5</v>
+      <c r="F14" s="14">
+        <v>5.5</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="14"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
@@ -999,14 +1299,18 @@
       <c r="D15" s="9">
         <v>6</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>5</v>
       </c>
-      <c r="F15" s="13">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="14"/>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
@@ -1018,14 +1322,18 @@
       <c r="D16" s="9">
         <v>8.5</v>
       </c>
-      <c r="E16" s="13">
-        <v>0</v>
-      </c>
-      <c r="F16" s="13">
+      <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
         <v>7</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="14"/>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
@@ -1037,12 +1345,14 @@
       <c r="D17" s="9">
         <v>20</v>
       </c>
-      <c r="E17" s="13">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="E17" s="12">
+        <v>0</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="14"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
@@ -1054,12 +1364,14 @@
       <c r="D18" s="9">
         <v>15</v>
       </c>
-      <c r="E18" s="13">
-        <v>0</v>
-      </c>
-      <c r="F18" s="9"/>
+      <c r="E18" s="12">
+        <v>0</v>
+      </c>
+      <c r="F18" s="12">
+        <v>1.25</v>
+      </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="14"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
@@ -1071,12 +1383,14 @@
       <c r="D19" s="9">
         <v>3</v>
       </c>
-      <c r="E19" s="13">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9"/>
+      <c r="E19" s="12">
+        <v>0</v>
+      </c>
+      <c r="F19" s="12">
+        <v>2</v>
+      </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
@@ -1088,12 +1402,14 @@
       <c r="D20" s="9">
         <v>3</v>
       </c>
-      <c r="E20" s="13">
-        <v>0</v>
-      </c>
-      <c r="F20" s="9"/>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="12">
+        <v>2</v>
+      </c>
       <c r="G20" s="9"/>
-      <c r="H20" s="14"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
@@ -1105,12 +1421,14 @@
       <c r="D21" s="9">
         <v>3</v>
       </c>
-      <c r="E21" s="13">
-        <v>0</v>
-      </c>
-      <c r="F21" s="9"/>
+      <c r="E21" s="12">
+        <v>0</v>
+      </c>
+      <c r="F21" s="12">
+        <v>2</v>
+      </c>
       <c r="G21" s="9"/>
-      <c r="H21" s="14"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
@@ -1122,12 +1440,14 @@
       <c r="D22" s="9">
         <v>3</v>
       </c>
-      <c r="E22" s="13">
-        <v>0</v>
-      </c>
-      <c r="F22" s="9"/>
+      <c r="E22" s="12">
+        <v>0</v>
+      </c>
+      <c r="F22" s="12">
+        <v>2</v>
+      </c>
       <c r="G22" s="9"/>
-      <c r="H22" s="14"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
@@ -1139,12 +1459,14 @@
       <c r="D23" s="9">
         <v>3</v>
       </c>
-      <c r="E23" s="13">
-        <v>0</v>
-      </c>
-      <c r="F23" s="9"/>
+      <c r="E23" s="12">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>2</v>
+      </c>
       <c r="G23" s="9"/>
-      <c r="H23" s="14"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
@@ -1156,12 +1478,14 @@
       <c r="D24" s="9">
         <v>3</v>
       </c>
-      <c r="E24" s="13">
-        <v>0</v>
-      </c>
-      <c r="F24" s="9"/>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>2</v>
+      </c>
       <c r="G24" s="9"/>
-      <c r="H24" s="14"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
@@ -1173,14 +1497,14 @@
       <c r="D25" s="9">
         <v>12</v>
       </c>
-      <c r="E25" s="13">
-        <v>0</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0</v>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0.75</v>
       </c>
       <c r="G25" s="9"/>
-      <c r="H25" s="14"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
@@ -1192,14 +1516,14 @@
       <c r="D26" s="9">
         <v>4</v>
       </c>
-      <c r="E26" s="13">
-        <v>0</v>
-      </c>
-      <c r="F26" s="13">
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
         <v>0</v>
       </c>
       <c r="G26" s="9"/>
-      <c r="H26" s="14"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
@@ -1209,39 +1533,39 @@
         <v>19</v>
       </c>
       <c r="D27" s="9">
-        <v>51</v>
-      </c>
-      <c r="E27" s="13">
+        <v>50</v>
+      </c>
+      <c r="E27" s="12">
         <v>1.5</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F27" s="12">
         <v>5</v>
       </c>
       <c r="G27" s="9"/>
-      <c r="H27" s="14"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="16">
+      <c r="D28" s="15">
         <f>D27+D26+D25+D24+D23+D22+D21+D20+D18+D19+D17+D16+D15+D14+D13+D12+D11+D10+D9+D8+D7+D6+D5+D4+D3</f>
-        <v>229.5</v>
-      </c>
-      <c r="E28" s="16">
+        <v>228.5</v>
+      </c>
+      <c r="E28" s="15">
         <f>E27+E26+E25+E24+E23+E22+E21+E20+E18+E19+E17+E16+E15+E14+E13+E12+E11+E10+E9+E8+E7+E6+E5+E4+E3</f>
         <v>56.5</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="15">
         <f>F27+F26+F25+F24+F23+F22+F21+F20+F18+F19+F17+F16+F15+F14+F13+F12+F11+F10+F9+F8+F7+F6+F5+F4+F3</f>
-        <v>46.3</v>
-      </c>
-      <c r="G28" s="16">
+        <v>76.55</v>
+      </c>
+      <c r="G28" s="15">
         <f>G27+G26+G25+G24+G23+G22+G21+G20+G18+G19+G17+G16+G15+G14+G13+G12+G11+G10+G9+G8+G7+G6+G5+G4+G3</f>
         <v>0</v>
       </c>
-      <c r="H28" s="17">
+      <c r="H28" s="16">
         <f>H27+H26+H25+H24+H23+H22+H21+H20+H18+H19+H17+H16+H15+H14+H13+H12+H11+H10+H9+H8+H7+H6+H5+H4+H3</f>
         <v>0</v>
       </c>
@@ -1249,232 +1573,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0251FC6A-65FF-4A7A-8436-F3FD3989FCD1}">
-  <dimension ref="B1:C27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="16.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
-        <v>6</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>7</v>
-      </c>
-      <c r="C9" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>9</v>
-      </c>
-      <c r="C11" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>10</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>11</v>
-      </c>
-      <c r="C13" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="2">
-        <v>12</v>
-      </c>
-      <c r="C14" s="19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2">
-        <v>13</v>
-      </c>
-      <c r="C15" s="19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2">
-        <v>14</v>
-      </c>
-      <c r="C16" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" s="2">
-        <v>15</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" s="2">
-        <v>16</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B19" s="2">
-        <v>17</v>
-      </c>
-      <c r="C19" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B20" s="2">
-        <v>18</v>
-      </c>
-      <c r="C20" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B21" s="2">
-        <v>19</v>
-      </c>
-      <c r="C21" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B22" s="2">
-        <v>20</v>
-      </c>
-      <c r="C22" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="2">
-        <v>21</v>
-      </c>
-      <c r="C23" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B24" s="2">
-        <v>22</v>
-      </c>
-      <c r="C24" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B25" s="2">
-        <v>23</v>
-      </c>
-      <c r="C25" s="19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" s="2">
-        <v>24</v>
-      </c>
-      <c r="C26" s="19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="20">
-        <v>25</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de la validation des requêtes
</commit_message>
<xml_diff>
--- a/Docs/Analyse_Sanguine/Chemin critique.xlsx
+++ b/Docs/Analyse_Sanguine/Chemin critique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ecole\Projet Final\Rooftop\Docs\Analyse_Sanguine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A393D-A99A-4DEE-A2E6-550431C757AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0942787F-D41A-4027-9944-321D7D898934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7454C503-1B9C-4864-A7C2-5D0980A5147F}"/>
   </bookViews>
@@ -69,7 +69,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-L'avancement du API a bien avancée durant la semaine et celui-ci est fonctionnel, ainsi nous avons atteint ce que nous nous attendions de faire cette semaine</t>
+L'avancement du API a bien avancée durant la semaine et celui-ci est quasi fonctionnel.
+Nous nous attendions de faire environ 16h pour l'API pour le terminé cette semaine et étant donné que celui-ci est quasi fonctionnel en 9h, le temps restant, même si beaucoup plus grand car nous avons terminé l'API en moins de temps que prévu, permettera de modifier celui-ci si des problèmes futurs surviennent.</t>
         </r>
       </text>
     </comment>
@@ -93,7 +94,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Le travail était en moyenne très bien, les interfaces pour les controlleurs étaient bien, cependant quelques inconvénients ont été rencontrés durant l'ajout de seed.</t>
+          <t>Le travail était en moyenne très bien, les interfaces pour les controlleurs étaient bien, cependant quelques inconvénients ont été rencontrés durant l'ajout de seed.
+Avec le temps restant sur l'API d'environ 7h que nous avons prédit faire cette semaine, nous n'avons pas réussi à rester dans les temps que nous nous avions donné pour terminé la tâche. Cette échec viens surtout du seed qui a prit beaucoup plus que temps que prévus pour régler les problèmes de migrations et a grandement allongés le temps pour terminé cette tâche.</t>
         </r>
       </text>
     </comment>
@@ -117,7 +119,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Même si l'avancement du cas d'utilisation est relativement lent, le formulaire reste créer et le cas d'utilisation à permis à Maxime d'apprendre à faire des components react-native, ainsi le temps prit peut être justifié à cause de l'apprentissage qui venait avec.</t>
+          <t>Même si l'avancement du cas d'utilisation est relativement lent, le formulaire reste créer et le cas d'utilisation à permis à Maxime d'apprendre à faire des components react-native, ainsi le temps prit peut être justifié à cause de l'apprentissage qui venait avec.
+Ainsi, le temps que nous avons prédit que cette tâche prendrait cette semaine de 7h à clairement été dépassé. Il peut être dit que ce dépassement est arrivé à cause de l'apprentissage d'un nouveau language que nous avons clairement sous-estimé le temps requis pour l'apprendre et l'utilisé efficacement.</t>
         </r>
       </text>
     </comment>
@@ -142,7 +145,82 @@
             <family val="2"/>
           </rPr>
           <t>La création du formulaire est fonctionnel, même s'il n'est pas terminé, une requête peut belle et bien être créé. Certaine type de test ne sont pas 100% fonctionnel, mais la majorité reste finit.
-L'excès de temps vient surtout du fait que le nombre de test ont clairement été sous-estimé de notre part, ainsi nous aurions dû prévoir plus de temps pour conclure la tâche.</t>
+Étant donné que la semaine derrière nous avons prit un excès de temps pour la tâche, il restait logiquement 10h30 a mettre dans la tâche pour la terminé, un temps qui a clairmenet été dépassé de 54 minutes et la tâche n'est pas totalement terminé. Ce grand excès peut être vu à cause de la grandeur des types de test possible qui était clairement sous-estimé.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{BE67C652-392A-4032-BA63-310D1C627FC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Créer la requête : (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+…
+Nous prévoyons que pour terminé cette tâche qui dépasse déjà nos attentes, nous allons prendre 11h pour terminé la tâche, ...</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{3E219063-5BFD-4E35-BB9A-54B478568037}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Visualiser les requêtes: (En dev.)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Le développement des requêtes avancent biens, l'affichage est totalement fini et tout ce qui devrait rester est de fetch l'API.
+Pour ce développement de 5h, nous avons prévu que nous allons prendre environ 3h pour faire le visuel ce temps à quasiment été respecté avec un 30 minutes de moins. Nous pensions que le visuel allait prendre plus de temps, car ce type de visuel n'avait jamais été fait auparavant dans notre parcours (React-Native)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{9A25B938-9563-43FC-8DAB-1F7D51B7DFF9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Visualiser les requêtes: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+L'avancement et la finition de la tâche a été bien cette semaine, même si un peu plus rapidement que prévu.
+Étant donné la durée de la tâche prévu et le temps fait la semaine dernière, le nombre de temps cette semaine aurait dû être de 2h30. Étant donné que la tâche à été réaliser sans grand problème, le fetch vers l'API a prit le temps que nous avons initialement prévu, c'est à dire 2h.</t>
         </r>
       </text>
     </comment>
@@ -166,7 +244,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Le travail effectué sur la création de requête était très peu productive cette semaine. Le temps prit était énorme en comparaison au travail qui a été effectué (seulement le visuel). La lenteur est venu principalement du bouton qui amène au formulaire.</t>
+          <t>Le travail effectué sur la création de requête était très peu productive cette semaine. Le temps prit était énorme en comparaison au travail qui a été effectué (seulement le visuel). La lenteur est venu principalement du bouton qui amène au formulaire.
+Le temps prévus pour la tâche cette semaine d'environ 8h n'a pas été respecté. Cette excès de temps peut être vu à cause du temps mis pour le bouton qui permet d'accéder au formulaire de création qui a été beaucoup trop grand (~4h30)</t>
         </r>
       </text>
     </comment>
@@ -240,7 +319,32 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-La modification du dossier a été un cas d'utilisation qui c'est très bien déroulé. La durée a été dans les temps que nous avons prédis et il restait du temps si nous avons rencontré plus de problème.</t>
+La modification du dossier a été un cas d'utilisation qui c'est très bien déroulé. La durée a été dans les temps que nous avons prédis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{B5D33080-C901-4BB9-9CAF-D61EB8FE6BFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Visualiser un résultat: (En dev.)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+L'avancement effectué viens surtout de l'installation du module de tableau et de l'apprentissge pour l'utiliser. Ainsi même si le cas d'utilisations a été avancé, l'avancement n'est pas vraiment significatif.
+Nous n'avons pas prévu travaillé sur ce cas d'utilisation cette semaine, ainsi le temps utilisé pour cette apprentisage dépasse un peu ce que nous avons attendu.</t>
         </r>
       </text>
     </comment>
@@ -254,7 +358,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>API Test: (Terminé)</t>
+          <t>API Test: (En dev.)</t>
         </r>
         <r>
           <rPr>
@@ -265,7 +369,33 @@
           </rPr>
           <t xml:space="preserve">
 Les test de l'API ont été terminés dans un délais de temps relativement faible tout en étant fonctionnel dans la très grande majorité.
-Ainsi, ses cas d'utilisations ont été terminés dans un délais que nous nous attendions.</t>
+Ainsi, les cas d'utilisations ce sont terminés dans des délais un peu plus petit que prévus (1h). Les problèmes que nous avons prédit arrivé n'ont pas survenu.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{15AD6CA3-0960-4460-80F7-FF066CC0DA3A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>API Test: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+…
+...</t>
         </r>
       </text>
     </comment>
@@ -403,7 +533,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,8 +575,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,6 +602,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -652,7 +795,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -678,6 +821,8 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,7 +1140,7 @@
   <dimension ref="B1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,13 +1214,13 @@
       <c r="E4" s="12">
         <v>1.5</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="14">
         <v>2</v>
       </c>
-      <c r="G4" s="12">
-        <v>0</v>
-      </c>
-      <c r="H4" s="20">
+      <c r="G4" s="14">
+        <v>0</v>
+      </c>
+      <c r="H4" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1110,18 +1255,18 @@
         <v>6</v>
       </c>
       <c r="D6" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E6" s="12">
         <v>1.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="14">
         <v>4.25</v>
       </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20">
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1133,18 +1278,18 @@
         <v>7</v>
       </c>
       <c r="D7" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7" s="12">
         <v>1.5</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="14">
         <v>4.25</v>
       </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="20">
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18">
         <v>0</v>
       </c>
     </row>
@@ -1187,8 +1332,10 @@
       <c r="F9" s="14">
         <v>10.9</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
@@ -1198,16 +1345,20 @@
         <v>9</v>
       </c>
       <c r="D10" s="9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E10" s="12">
         <v>2.5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="21">
         <v>2</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="13"/>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
@@ -1222,11 +1373,15 @@
       <c r="E11" s="12">
         <v>2.5</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="14">
         <v>6.75</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="13"/>
+      <c r="G11" s="14">
+        <v>0</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
@@ -1264,11 +1419,15 @@
       <c r="E13" s="12">
         <v>11.5</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="21">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="13"/>
+      <c r="G13" s="21">
+        <v>0</v>
+      </c>
+      <c r="H13" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
@@ -1286,8 +1445,12 @@
       <c r="F14" s="14">
         <v>5.5</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="13"/>
+      <c r="G14" s="14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
@@ -1299,16 +1462,16 @@
       <c r="D15" s="9">
         <v>6</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="21">
         <v>5</v>
       </c>
-      <c r="F15" s="12">
-        <v>0</v>
-      </c>
-      <c r="G15" s="12">
-        <v>0</v>
-      </c>
-      <c r="H15" s="20">
+      <c r="F15" s="21">
+        <v>0</v>
+      </c>
+      <c r="G15" s="21">
+        <v>0</v>
+      </c>
+      <c r="H15" s="22">
         <v>0</v>
       </c>
     </row>
@@ -1320,7 +1483,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="9">
-        <v>8.5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
@@ -1343,7 +1506,7 @@
         <v>17</v>
       </c>
       <c r="D17" s="9">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -1362,7 +1525,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="9">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E18" s="12">
         <v>0</v>
@@ -1386,11 +1549,15 @@
       <c r="E19" s="12">
         <v>0</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="21">
         <v>2</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="13"/>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
@@ -1408,8 +1575,12 @@
       <c r="F20" s="12">
         <v>2</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="13"/>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
@@ -1424,11 +1595,15 @@
       <c r="E21" s="12">
         <v>0</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="21">
         <v>2</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="13"/>
+      <c r="G21" s="21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
@@ -1443,11 +1618,15 @@
       <c r="E22" s="12">
         <v>0</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="21">
         <v>2</v>
       </c>
-      <c r="G22" s="9"/>
-      <c r="H22" s="13"/>
+      <c r="G22" s="21">
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
@@ -1462,11 +1641,15 @@
       <c r="E23" s="12">
         <v>0</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="21">
         <v>2</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="13"/>
+      <c r="G23" s="21">
+        <v>0</v>
+      </c>
+      <c r="H23" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
@@ -1481,11 +1664,15 @@
       <c r="E24" s="12">
         <v>0</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="21">
         <v>2</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="13"/>
+      <c r="G24" s="21">
+        <v>0</v>
+      </c>
+      <c r="H24" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
@@ -1551,7 +1738,7 @@
       </c>
       <c r="D28" s="15">
         <f>D27+D26+D25+D24+D23+D22+D21+D20+D18+D19+D17+D16+D15+D14+D13+D12+D11+D10+D9+D8+D7+D6+D5+D4+D3</f>
-        <v>228.5</v>
+        <v>209</v>
       </c>
       <c r="E28" s="15">
         <f>E27+E26+E25+E24+E23+E22+E21+E20+E18+E19+E17+E16+E15+E14+E13+E12+E11+E10+E9+E8+E7+E6+E5+E4+E3</f>
@@ -1563,7 +1750,7 @@
       </c>
       <c r="G28" s="15">
         <f>G27+G26+G25+G24+G23+G22+G21+G20+G18+G19+G17+G16+G15+G14+G13+G12+G11+G10+G9+G8+G7+G6+G5+G4+G3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="16">
         <f>H27+H26+H25+H24+H23+H22+H21+H20+H18+H19+H17+H16+H15+H14+H13+H12+H11+H10+H9+H8+H7+H6+H5+H4+H3</f>

</xml_diff>

<commit_message>
Continuation de la doc
</commit_message>
<xml_diff>
--- a/Docs/Analyse_Sanguine/Chemin critique.xlsx
+++ b/Docs/Analyse_Sanguine/Chemin critique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ecole\Projet Final\Rooftop\Docs\Analyse_Sanguine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0942787F-D41A-4027-9944-321D7D898934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFC488E-342F-41B8-B2EC-7FBE960F8BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7454C503-1B9C-4864-A7C2-5D0980A5147F}"/>
   </bookViews>
@@ -224,6 +224,56 @@
         </r>
       </text>
     </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{47A9FCA0-83FB-4DDE-9E72-917A79A98177}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Visualiser une requête: (En dev.)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La visualiton d'une requête à eu un bon avancement cette semaine. L'affichage en loi même est terminé comme nous le désirons et il ne restera que le relié avec l'API et corrigé quelques petits problèmes qui peut surgir.
+Le temps prévu pour cette tâche cette semaine était d'environ 3h, ainsi nous sommes restés dans les alentours du temps prévues. Nous pensions que le visuel allait être un peu plus complexe à réaliser, mais pour la visualisation d'une requête, le visuel a été relativement simple à faire.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{EB2B93A7-3A44-41CF-BCA2-605A25AB046E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Visualiser une requête: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Avec l'arrivé de l'API qui était fonctionnel ainsi que les résultats d'analyse que nous devions faire, la visualiser d'une requête est devenu beaucoup plus complexe que nous l'avions initialement prévue. Même si nous avons réussi à le terminé, le cas d'utilisation à prit beaucoup plus de temps que nous l'avons prévus à cause de léger problème avec l'API, mais surtout à cause du nombre de type d'analyse que nous devions mettre dans l'application.
+Le temps prévus à la tâche était d'environ 4h30 cette semaine, ce qui a été largement dépassé de 2h15. Un grand excès qui peut être vu, comme dit plus haut, par la sous-estimation du nombre d'analyse qui était requis pour les requêtes.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="E12" authorId="0" shapeId="0" xr:uid="{2D2B52A4-1255-4B7F-8805-DD8BAC12CC90}">
       <text>
         <r>
@@ -270,7 +320,107 @@
             <family val="2"/>
           </rPr>
           <t>L'avancement fait cette semaine sur la création de dossier était beaucoup plus productif cette semaine. Le formulaire a pu être terminé et même si le temps a été dépassé 2h45, l'avancement fait a été plus rapide qu'auparavant.
-De cette manière, l'excès de temps peut être vu à cause des problèmes avec l'accès au API qui est arrivé dans ce cas d'utilisation. Le bouton pour la création reste la cause principale de l'excès de temps</t>
+De cette manière, l'excès de temps peut être vu à cause des problèmes avec l'accès au API qui sont arrivés dans ce cas d'utilisation. Le bouton pour la création reste la cause principale de l'excès de temps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{26452CEB-B184-4D65-B9C0-2735BE532F94}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Visualiser les dossiers: (En dev.)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Étant donné que ce cas d'utilisation visuel était le premier qui devait être fait, nous avions prévus que celui-ci allait prendre beaucoup de temps cette semaine et le temps utilisé de 11h30 à respecter cette échéancier tout en permettant de l'avancée à un bon rythme.
+Nous avions prévus travaillé sur ce cas d'utilisation environ 11h à 12h cette semaine, un temps qui a été respecté tout en finissant le visuel de la liste.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{B6CADD2E-ECF2-42CA-8C39-7E39D97D89B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Visualiser les dossiers: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Le cas d'utilisation a été terminé dans un temps très raisonnable tout en étant ce que nous nous attendions à avoir.
+Nous avions prévus travaillé environ 3h sur ce cas d'utilisation pour faire l'appel à l'API et les problèmes qui pouvait subvenir avec cette appel. Même si nous avons réussis à terminé le cas, sa finition à été clairement plus petite que ce que nous avons prévus (1h45 de moins). La sous-estimation de temps peut être vu à cause du nombre de temps que l'API nous as prit dans les autres tâches, ce qui nous a influencé à estimé une plus grande durée pour ce cas d'utilisation.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{55F8B0AE-D90A-4960-9266-46552A2DA0AC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Visualiser un dossier: (En dev.)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Le cas d'utilisation, même si son avancement est bon, nous a prit trop de temps pour ce que nous nous attendions à prendre.
+Nous avons estimé que le temps requis pour ce cas cette semaine serait de 4h, un temps qui a été dépassé de 30 minutes. Cette excès de temps peut être venu du fait que nous apprenions le language utilisé et que cet apprentisage à prit plus de temps que nous l'avions initialement prévus.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{3CB91BC0-2EAF-430A-951A-4C316F73C74E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Visualiser un dossier: (Terminé)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ce cas d'utilisation à prit beaucoup plus de temps que nous l'avons initialement prévu et même s'il est terminé, nous n'avons passé trop de temps à le finir.
+Le temps prévus pour effectué cette tâche cette semaine était d'environ 1h30, un temps qui a été plus que doublé. Cet excès de temps peut être remarqué à cause de la difficulté de l'API qui a influencé plusieurs tâches de l'application.</t>
         </r>
       </text>
     </comment>
@@ -394,8 +544,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-…
-...</t>
+Les tests de l'API ont été terminés facilement et efficacement cette semaine. 
+Le temps estimé de 1h pour terminé le test restant des requêtes à été respecté ce qui a permis à ce test d'être dans les temps que nous avons prévus initialement.</t>
         </r>
       </text>
     </comment>
@@ -1139,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5812C443-2D11-4192-ADEE-E8DB4E96BFCE}">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,8 +1840,12 @@
       <c r="F25" s="12">
         <v>0.75</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="13"/>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
@@ -1728,8 +1882,12 @@
       <c r="F27" s="12">
         <v>5</v>
       </c>
-      <c r="G27" s="9"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3"/>

</xml_diff>